<commit_message>
Wheelchair BOM Revision 2012A
</commit_message>
<xml_diff>
--- a/hardware/Connector BOM.xlsx
+++ b/hardware/Connector BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="109">
   <si>
     <t>Photointerrupter</t>
   </si>
@@ -353,6 +353,18 @@
   </si>
   <si>
     <t>538-46012-3142</t>
+  </si>
+  <si>
+    <t>538-39-01-2240</t>
+  </si>
+  <si>
+    <t>39-01-2240</t>
+  </si>
+  <si>
+    <t>D-sub standoffs</t>
+  </si>
+  <si>
+    <t>93620A701</t>
   </si>
 </sst>
 </file>
@@ -737,11 +749,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +852,7 @@
         <v>4</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I3:I33" si="0">G3*H3</f>
+        <f t="shared" ref="I3:I34" si="0">G3*H3</f>
         <v>18.84</v>
       </c>
     </row>
@@ -1219,9 +1231,27 @@
       <c r="B17" t="s">
         <v>82</v>
       </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
       <c r="I17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1601,9 +1631,30 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
       <c r="I34" s="3">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="3">
         <f>SUM(I2:I33)</f>
-        <v>302.81299999999993</v>
+        <v>304.06299999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remote software compensates for sheared joystick axes
</commit_message>
<xml_diff>
--- a/hardware/Connector BOM.xlsx
+++ b/hardware/Connector BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="110">
   <si>
     <t>Photointerrupter</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Disconnect housing</t>
   </si>
   <si>
-    <t>Disconnect contact</t>
-  </si>
-  <si>
     <t>879-6810G1-BK</t>
   </si>
   <si>
@@ -59,13 +56,7 @@
     <t>879-1321-BK</t>
   </si>
   <si>
-    <t>Panel mount contact</t>
-  </si>
-  <si>
     <t>879-1464G2</t>
-  </si>
-  <si>
-    <t>Additional contact</t>
   </si>
   <si>
     <t>879-1319G4-BK</t>
@@ -283,9 +274,6 @@
     <t>Panel mount (pair)</t>
   </si>
   <si>
-    <t>Panel mount plates (single?)</t>
-  </si>
-  <si>
     <t>Plug</t>
   </si>
   <si>
@@ -365,6 +353,21 @@
   </si>
   <si>
     <t>93620A701</t>
+  </si>
+  <si>
+    <t>Panel mount plates (pair - complain to Mouser if single)</t>
+  </si>
+  <si>
+    <t>Panel mount contact 6 AWG</t>
+  </si>
+  <si>
+    <t>Disconnect contact 6 AWG</t>
+  </si>
+  <si>
+    <t>Additional contact 4 AWG</t>
+  </si>
+  <si>
+    <t>Additional contact 2 AWG</t>
   </si>
 </sst>
 </file>
@@ -753,13 +756,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23:E32"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
@@ -771,16 +774,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -789,33 +792,33 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G2" s="3">
         <v>0.66</v>
@@ -834,16 +837,16 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="3">
         <v>4.71</v>
@@ -859,19 +862,19 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3">
         <v>3.26</v>
@@ -887,19 +890,19 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
       </c>
       <c r="G5" s="3">
         <v>4.95</v>
@@ -915,19 +918,19 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="3">
         <v>3.26</v>
@@ -943,19 +946,19 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G7" s="3">
         <v>7.04</v>
@@ -971,77 +974,77 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G8" s="3">
         <v>3.14</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="0"/>
-        <v>6.28</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G9" s="3">
         <v>3.14</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I9" s="3">
         <f>G9*H9</f>
-        <v>6.28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G10" s="3">
         <v>1.47</v>
@@ -1057,19 +1060,19 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G11" s="3">
         <v>1.47</v>
@@ -1085,19 +1088,19 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G12" s="3">
         <v>0.62</v>
@@ -1113,19 +1116,19 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G13" s="3">
         <v>4.1900000000000004</v>
@@ -1143,19 +1146,19 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G14" s="3">
         <v>1.86</v>
@@ -1171,19 +1174,19 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G15" s="3">
         <v>2.54</v>
@@ -1198,22 +1201,22 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G16" s="3">
         <v>2.0699999999999998</v>
@@ -1229,19 +1232,19 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G17" s="3">
         <v>1.25</v>
@@ -1257,19 +1260,19 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
         <v>99</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" t="s">
-        <v>103</v>
       </c>
       <c r="G18" s="3">
         <v>8.5000000000000006E-2</v>
@@ -1285,19 +1288,19 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
         <v>100</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" t="s">
-        <v>104</v>
       </c>
       <c r="G19" s="3">
         <v>0.222</v>
@@ -1315,19 +1318,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G20" s="3">
         <v>3.32</v>
@@ -1343,19 +1346,19 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
         <v>67</v>
-      </c>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" t="s">
-        <v>70</v>
       </c>
       <c r="G21" s="3">
         <v>3.19</v>
@@ -1373,7 +1376,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I22" s="3">
         <f t="shared" si="0"/>
@@ -1382,16 +1385,16 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G23" s="3">
         <v>1.68</v>
@@ -1407,13 +1410,13 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G24" s="3">
         <v>1.68</v>
@@ -1429,13 +1432,13 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G25" s="3">
         <v>1.18</v>
@@ -1451,13 +1454,13 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G26" s="3">
         <v>1.18</v>
@@ -1473,13 +1476,13 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G27" s="3">
         <f>9.19/100</f>
@@ -1496,13 +1499,13 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G28" s="3">
         <f>9.19/100</f>
@@ -1519,13 +1522,13 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G29" s="3">
         <f>22.87/100</f>
@@ -1542,13 +1545,13 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E30" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F30" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G30" s="3">
         <f>22.87/100</f>
@@ -1565,13 +1568,13 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G31" s="3">
         <v>0.22869999999999999</v>
@@ -1587,13 +1590,13 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G32" s="3">
         <v>1.47</v>
@@ -1608,16 +1611,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G33" s="3">
         <v>7.95</v>
@@ -1632,13 +1635,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F34" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G34" s="3">
         <v>1.4</v>
@@ -1654,7 +1657,7 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I35" s="3">
         <f>SUM(I2:I33)</f>
-        <v>304.06299999999993</v>
+        <v>294.64299999999992</v>
       </c>
     </row>
   </sheetData>
@@ -1690,7 +1693,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
@@ -1699,30 +1702,30 @@
         <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E2" s="7">
         <v>1.68</v>
@@ -1738,13 +1741,13 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7">
         <v>1.68</v>
@@ -1760,13 +1763,13 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E4" s="7">
         <v>1.18</v>
@@ -1782,13 +1785,13 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E5" s="7">
         <v>1.18</v>
@@ -1803,16 +1806,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E6" s="7">
         <v>7.95</v>

</xml_diff>